<commit_message>
updated Table S2 and S3 and Fig 6
</commit_message>
<xml_diff>
--- a/1_Overview/Table S2 Sorting conditions.xlsx
+++ b/1_Overview/Table S2 Sorting conditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattsmith/Dropbox (University of Michigan)/from_box/My_Stuff/Python_Codes/mds_pkgs/TessierLab Github/PSERM_Paper/PSERM_paper/1_Overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD65FFC-C6BE-F24C-AA4B-5E4CF45873AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B502F351-C358-F64B-8C4B-98FB5B684337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16940" xr2:uid="{772DA7F5-EC53-7F4D-A638-18946D88480A}"/>
+    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="16940" xr2:uid="{772DA7F5-EC53-7F4D-A638-18946D88480A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
   <si>
     <t>Project</t>
   </si>
@@ -47,12 +47,6 @@
     <t>Sample</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Input</t>
-  </si>
-  <si>
     <t>Dataset 1</t>
   </si>
   <si>
@@ -192,9 +186,6 @@
   </si>
   <si>
     <t>Reagent</t>
-  </si>
-  <si>
-    <t>100x dilutoin of QD-lenzilumab</t>
   </si>
   <si>
     <t>1 hr</t>
@@ -256,12 +247,15 @@
       <t xml:space="preserve"> coated dynabeads</t>
     </r>
   </si>
+  <si>
+    <t>100x dilution of QD-lenzilumab</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -283,11 +277,6 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="MyriadPro-Regular"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
@@ -322,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -413,19 +402,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="medium">
@@ -464,11 +440,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -476,12 +472,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -490,56 +480,75 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -855,520 +864,443 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A73851-3D59-6344-BEBB-4D8EEC971ACC}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I21"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="33" thickBot="1">
-      <c r="A2" s="7"/>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="5"/>
+      <c r="B3" s="17">
+        <v>1</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="H3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="5"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="5"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="5"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" ht="16" customHeight="1">
+      <c r="A7" s="5"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="5"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="5"/>
+      <c r="B9" s="17">
+        <v>2</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="5"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" ht="16" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="7"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="7"/>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="5"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="5"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="5"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" ht="19" customHeight="1">
+      <c r="A15" s="5"/>
+      <c r="B15" s="17">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="7"/>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="7"/>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="7"/>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="7"/>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="1:10" ht="16" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="20" t="s">
+      <c r="C15" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="7"/>
-      <c r="B9" s="4">
-        <v>1</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="7"/>
-      <c r="B10" s="3">
-        <v>2</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="7"/>
-      <c r="B11" s="3">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="J11" s="7"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="7"/>
-      <c r="B12" s="3">
-        <v>2</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="7"/>
-    </row>
-    <row r="13" spans="1:10" ht="16" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="3">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="22" t="s">
+      <c r="I15" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="J13" s="7"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="7"/>
-      <c r="B14" s="3">
-        <v>2</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="7"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="7"/>
-      <c r="B15" s="3">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="J15" s="7"/>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="7"/>
-      <c r="B16" s="4">
-        <v>2</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="7"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="7"/>
-      <c r="B17" s="3">
-        <v>3</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="7"/>
-    </row>
-    <row r="18" spans="1:10" ht="19" customHeight="1">
-      <c r="A18" s="7"/>
-      <c r="B18" s="3">
-        <v>3</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="I18" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="J18" s="7"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="5"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="7"/>
-      <c r="B19" s="3">
-        <v>3</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="7"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="7"/>
-      <c r="B20" s="3">
-        <v>3</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="7"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="7"/>
-      <c r="B21" s="3">
-        <v>3</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="7"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="E26" s="8"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="E23" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="30">
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="F9:F10"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="I18:I21"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="E3:E9"/>
-    <mergeCell ref="E10:E16"/>
-    <mergeCell ref="E17:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updates with supplemental figures
</commit_message>
<xml_diff>
--- a/1_Overview/Table S2 Sorting conditions.xlsx
+++ b/1_Overview/Table S2 Sorting conditions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattsmith/Dropbox (University of Michigan)/from_box/My_Stuff/Python_Codes/mds_pkgs/TessierLab Github/PSERM_Paper/PSERM_paper/1_Overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B502F351-C358-F64B-8C4B-98FB5B684337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCA7665-28C5-8748-85DF-26E3EAD4158E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="16940" xr2:uid="{772DA7F5-EC53-7F4D-A638-18946D88480A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
   <si>
     <t>Project</t>
   </si>
@@ -155,9 +155,6 @@
     <t>Incubation time</t>
   </si>
   <si>
-    <t>3 hr</t>
-  </si>
-  <si>
     <t>Buffer conditions</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>Reagent</t>
   </si>
   <si>
-    <t>1 hr</t>
-  </si>
-  <si>
     <t>0.1x PBS + 0.1% BSA</t>
   </si>
   <si>
@@ -204,9 +198,6 @@
   </si>
   <si>
     <t>500 nM LPLA2</t>
-  </si>
-  <si>
-    <t>1.5 hr</t>
   </si>
   <si>
     <r>
@@ -249,6 +240,15 @@
   </si>
   <si>
     <t>100x dilution of QD-lenzilumab</t>
+  </si>
+  <si>
+    <t>3 h</t>
+  </si>
+  <si>
+    <t>1 h</t>
+  </si>
+  <si>
+    <t>1.5 h</t>
   </si>
 </sst>
 </file>
@@ -311,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -441,21 +441,36 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
         <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -481,74 +496,78 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -867,7 +886,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="I15" sqref="I15:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -896,38 +915,38 @@
     </row>
     <row r="2" spans="1:10" ht="33" thickBot="1">
       <c r="A2" s="5"/>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="32" t="s">
-        <v>40</v>
+      <c r="H2" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="5"/>
-      <c r="B3" s="17">
+      <c r="B3" s="20">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="18" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -937,253 +956,247 @@
         <v>4</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>50</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="5"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="F4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="23"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="5"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="15"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="25" t="s">
-        <v>53</v>
+      <c r="F5" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>51</v>
       </c>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="5"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="15"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="23"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" ht="16" customHeight="1">
       <c r="A7" s="5"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="15"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>53</v>
+      <c r="H7" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>51</v>
       </c>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="5"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="16"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="13"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="23"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="5"/>
-      <c r="B9" s="17">
+      <c r="B9" s="20">
         <v>2</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="18" t="s">
         <v>35</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="11" t="s">
+      <c r="F9" s="29" t="s">
         <v>52</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>50</v>
       </c>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="5"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="15"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="13"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="23"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" ht="16" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="15"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="18"/>
       <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" s="25" t="s">
-        <v>51</v>
+      <c r="F11" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="5"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="15"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="13"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="23"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="5"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="15"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>51</v>
+      <c r="F13" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" s="22" t="s">
+        <v>49</v>
       </c>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="5"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="16"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="13"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="23"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="19" customHeight="1">
       <c r="A15" s="5"/>
-      <c r="B15" s="17">
+      <c r="B15" s="20">
         <v>3</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="18" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1192,66 +1205,66 @@
       <c r="E15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>52</v>
+      <c r="F15" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>50</v>
       </c>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="5"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="15"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="11"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="22"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="5"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="15"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="18"/>
       <c r="D17" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="11"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="22"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="5"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="15"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="11"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="22"/>
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10">
@@ -1270,13 +1283,18 @@
       <c r="E23" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="B15:B18"/>
+  <mergeCells count="33">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="I11:I12"/>
@@ -1287,20 +1305,18 @@
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="F11:F12"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="B15:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>